<commit_message>
Added mass balance checks to spreadsheet. Added OpenOffice Calc spreadsheet.
</commit_message>
<xml_diff>
--- a/Work/Excel/gx-fba examples.xlsx
+++ b/Work/Excel/gx-fba examples.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>glc_c</t>
   </si>
@@ -159,9 +159,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>FBAsolution</t>
-  </si>
-  <si>
     <t>Objectivevalue:</t>
   </si>
   <si>
@@ -183,7 +180,43 @@
     <t>GX-FBA UB</t>
   </si>
   <si>
-    <t xml:space="preserve">FAME </t>
+    <t>CobraPy FBAsolution</t>
+  </si>
+  <si>
+    <t>FAME FBA solution</t>
+  </si>
+  <si>
+    <t>CobraPy gx-FBA solution</t>
+  </si>
+  <si>
+    <t>FAME gx-FBA solution</t>
+  </si>
+  <si>
+    <t>Dumpedmodel:</t>
+  </si>
+  <si>
+    <t>gxfba_example:</t>
+  </si>
+  <si>
+    <t>Objective value</t>
+  </si>
+  <si>
+    <t>Objective coefficients</t>
+  </si>
+  <si>
+    <t>Mass balance checks:</t>
+  </si>
+  <si>
+    <t>2V1 - V3 - V7 - V8 - V13 = 0</t>
+  </si>
+  <si>
+    <t>2V1 -V5 - 2V7 - V8 - V13 = 0</t>
+  </si>
+  <si>
+    <t>4.5V2 -2V1 + 11.5V6 -10V8 = 12</t>
+  </si>
+  <si>
+    <t>V5 + 2V7 + V8 &lt;= 20</t>
   </si>
 </sst>
 </file>
@@ -224,10 +257,39 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -236,15 +298,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,15 +610,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:W44"/>
+  <dimension ref="A2:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
@@ -579,121 +643,122 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="W5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="V6" s="2">
+        <f>SUMPRODUCT(B6:U6,B$32:U$32)</f>
+        <v>-2.1521739130399999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>-1</v>
+      </c>
+      <c r="Q7">
+        <v>-1</v>
+      </c>
+      <c r="V7" s="2">
+        <f>SUMPRODUCT(B7:U7,B$32:U$32)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" ref="V8:V28" si="0">SUMPRODUCT(B8:U8,B$32:U$32)</f>
+        <v>-10</v>
+      </c>
+      <c r="W8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>-1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="V6" s="4">
-        <f>SUMPRODUCT(B6:U6,B$31:U$31)</f>
-        <v>-2.1521739130399999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>-1</v>
-      </c>
-      <c r="Q7">
-        <v>-1</v>
-      </c>
-      <c r="V7" s="4">
-        <f>SUMPRODUCT(B7:U7,B$31:U$31)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="V8" s="4">
-        <f t="shared" ref="V7:V30" si="0">SUMPRODUCT(B8:U8,B$31:U$31)</f>
-        <v>-10</v>
-      </c>
-      <c r="W8" t="s">
-        <v>50</v>
-      </c>
-    </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D9">
@@ -708,13 +773,13 @@
       <c r="P9">
         <v>-1</v>
       </c>
-      <c r="V9" s="4">
-        <f t="shared" si="0"/>
-        <v>299999.97000000003</v>
+      <c r="V9" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0217391304339998</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
       <c r="P10">
@@ -723,28 +788,28 @@
       <c r="R10">
         <v>-1</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="R11">
         <v>1</v>
       </c>
-      <c r="V11" s="4">
+      <c r="V11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C12">
@@ -762,13 +827,13 @@
       <c r="N12">
         <v>-1</v>
       </c>
-      <c r="V12" s="4">
-        <f t="shared" si="0"/>
-        <v>-99995.68565217391</v>
+      <c r="V12" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5869565217419996</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N13">
@@ -777,28 +842,28 @@
       <c r="S13">
         <v>-1</v>
       </c>
-      <c r="V13" s="4">
+      <c r="V13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="S14">
         <v>1</v>
       </c>
-      <c r="V14" s="4">
+      <c r="V14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D15">
@@ -816,34 +881,34 @@
       <c r="M15">
         <v>-1</v>
       </c>
-      <c r="V15" s="4">
-        <f t="shared" si="0"/>
-        <v>-99999.99</v>
+      <c r="V15" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.71739130434800003</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
-      <c r="V16" s="4">
+      <c r="V16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="V17" s="4">
+      <c r="V17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J18">
@@ -855,13 +920,13 @@
       <c r="O18">
         <v>-1</v>
       </c>
-      <c r="V18" s="4">
+      <c r="V18" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="O19">
@@ -870,28 +935,28 @@
       <c r="U19">
         <v>-1</v>
       </c>
-      <c r="V19" s="4">
+      <c r="V19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="7" t="s">
         <v>14</v>
       </c>
       <c r="U20">
         <v>1</v>
       </c>
-      <c r="V20" s="4">
+      <c r="V20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G21">
@@ -903,13 +968,13 @@
       <c r="K21">
         <v>-1</v>
       </c>
-      <c r="V21" s="4">
+      <c r="V21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G22">
@@ -921,13 +986,13 @@
       <c r="K22">
         <v>1</v>
       </c>
-      <c r="V22" s="4">
+      <c r="V22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B23">
@@ -945,13 +1010,13 @@
       <c r="J23">
         <v>-1</v>
       </c>
-      <c r="V23" s="4">
+      <c r="V23" s="2">
         <f t="shared" si="0"/>
         <v>3.0652173913249996</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B24">
@@ -969,13 +1034,13 @@
       <c r="J24">
         <v>1</v>
       </c>
-      <c r="V24" s="4">
+      <c r="V24" s="2">
         <f t="shared" si="0"/>
         <v>-3.0652173913249996</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B25">
@@ -984,13 +1049,13 @@
       <c r="C25">
         <v>-1</v>
       </c>
-      <c r="V25" s="4">
+      <c r="V25" s="2">
         <f t="shared" si="0"/>
         <v>-1.000000082740371E-11</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D26">
@@ -999,13 +1064,13 @@
       <c r="E26">
         <v>-1</v>
       </c>
-      <c r="V26" s="4">
-        <f t="shared" si="0"/>
-        <v>99999.99</v>
+      <c r="V26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.71739130434800003</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E27">
@@ -1017,13 +1082,13 @@
       <c r="H27">
         <v>-1</v>
       </c>
-      <c r="V27" s="4">
-        <f t="shared" si="0"/>
-        <v>-99999.99</v>
+      <c r="V27" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.65217391304299999</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="7" t="s">
         <v>27</v>
       </c>
       <c r="F28">
@@ -1032,14 +1097,14 @@
       <c r="G28">
         <v>-1</v>
       </c>
-      <c r="V28" s="4">
-        <f t="shared" si="0"/>
-        <v>99999.99</v>
+      <c r="V28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.65217391304299999</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1101,11 +1166,11 @@
       <c r="U29">
         <v>0</v>
       </c>
-      <c r="V29" s="4"/>
+      <c r="V29" s="2"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30">
         <v>99999.99</v>
@@ -1167,218 +1232,156 @@
       <c r="U30">
         <v>999999</v>
       </c>
-      <c r="V30" s="4"/>
+      <c r="V30" s="2"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="V31" s="2"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="3">
         <v>2.1521739130399999</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="3">
         <v>4.3043478260899999</v>
       </c>
-      <c r="D31" s="2">
-        <v>99999.99</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>99999.99</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
-      <c r="I31" s="3">
-        <v>0</v>
-      </c>
-      <c r="J31" s="2">
+      <c r="D32">
+        <v>0.71739130434800003</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0.65217391304299999</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
         <v>12</v>
       </c>
-      <c r="K31" s="2">
-        <v>0</v>
-      </c>
-      <c r="L31" s="2">
-        <v>0</v>
-      </c>
-      <c r="M31" s="2">
-        <v>0</v>
-      </c>
-      <c r="N31" s="2">
-        <v>0</v>
-      </c>
-      <c r="O31" s="2">
-        <v>0</v>
-      </c>
-      <c r="P31" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="2">
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
         <v>-10</v>
       </c>
-      <c r="R31" s="2">
-        <v>0</v>
-      </c>
-      <c r="S31" s="2">
-        <v>0</v>
-      </c>
-      <c r="T31" s="2">
-        <v>0</v>
-      </c>
-      <c r="U31" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>22</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>23</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>24</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>25</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>26</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" t="s">
         <v>28</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H33" t="s">
         <v>29</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J33" t="s">
         <v>31</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K33" t="s">
         <v>32</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L33" t="s">
         <v>33</v>
       </c>
-      <c r="M32" t="s">
+      <c r="M33" t="s">
         <v>34</v>
       </c>
-      <c r="N32" t="s">
+      <c r="N33" t="s">
         <v>35</v>
       </c>
-      <c r="O32" t="s">
+      <c r="O33" t="s">
         <v>36</v>
       </c>
-      <c r="P32" t="s">
+      <c r="P33" t="s">
         <v>37</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="Q33" t="s">
         <v>38</v>
       </c>
-      <c r="R32" t="s">
+      <c r="R33" t="s">
         <v>39</v>
       </c>
-      <c r="S32" t="s">
+      <c r="S33" t="s">
         <v>40</v>
       </c>
-      <c r="T32" t="s">
+      <c r="T33" t="s">
         <v>41</v>
       </c>
-      <c r="U32" t="s">
+      <c r="U33" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33">
-        <v>1.5</v>
-      </c>
-      <c r="C33">
-        <v>1.5</v>
-      </c>
-      <c r="D33">
-        <v>0.5</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0.5</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
-      <c r="R33">
-        <v>0</v>
-      </c>
-      <c r="S33">
-        <v>0</v>
-      </c>
-      <c r="T33">
-        <v>0</v>
-      </c>
-      <c r="U33">
-        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D34">
-        <v>0.71739130434800003</v>
+        <v>0.5</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0.65217391304299999</v>
+        <v>0.5</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1390,7 +1393,7 @@
         <v>0</v>
       </c>
       <c r="J34">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -1411,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="R34">
         <v>0</v>
@@ -1428,206 +1431,365 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35">
-        <v>2.1521739130399999</v>
-      </c>
-      <c r="C35">
-        <v>4.3043478260899999</v>
-      </c>
-      <c r="D35">
-        <v>99999.99</v>
-      </c>
-      <c r="E35">
-        <v>99999.99</v>
-      </c>
-      <c r="F35">
-        <v>99999.99</v>
-      </c>
-      <c r="G35">
-        <v>99999.99</v>
-      </c>
-      <c r="H35">
-        <v>99999.99</v>
-      </c>
-      <c r="I35">
-        <v>99999.99</v>
-      </c>
-      <c r="J35">
-        <v>12</v>
-      </c>
-      <c r="K35">
-        <v>99999.99</v>
-      </c>
-      <c r="L35">
-        <v>99999</v>
-      </c>
-      <c r="M35">
-        <v>99999.99</v>
-      </c>
-      <c r="N35">
-        <v>99999</v>
-      </c>
-      <c r="O35">
-        <v>99999.99</v>
-      </c>
-      <c r="P35">
-        <v>99999.99</v>
-      </c>
-      <c r="Q35">
-        <v>999999</v>
-      </c>
-      <c r="R35">
-        <v>999999</v>
-      </c>
-      <c r="S35">
-        <v>5</v>
-      </c>
-      <c r="T35">
-        <v>999999</v>
-      </c>
-      <c r="U35">
-        <v>999999</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36">
-        <f>SUMPRODUCT(B31:U31,B33:U33)</f>
-        <v>100009.67478260869</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37">
+        <f>SUMPRODUCT(B32:U32,B34:U34)</f>
+        <v>10.369565217390498</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39">
+      <c r="A39" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40">
         <v>1.4347826087</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>2.8695652173899999</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>1.4347826087</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>1.4347826087</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <v>1.3043478260900001</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>1.3043478260900001</v>
       </c>
-      <c r="H39">
+      <c r="H40">
         <v>0.13043478260899999</v>
       </c>
-      <c r="I39">
+      <c r="I40">
         <v>1.3043478260900001</v>
       </c>
-      <c r="J39">
+      <c r="J40">
         <v>12</v>
       </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
         <v>1.4347826087</v>
       </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39">
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
         <v>12</v>
       </c>
-      <c r="P39">
+      <c r="P40">
         <v>4.1739130434799998</v>
       </c>
-      <c r="Q39">
+      <c r="Q40">
         <v>-1.4347826087</v>
       </c>
-      <c r="R39">
+      <c r="R40">
         <v>4.1739130434799998</v>
       </c>
-      <c r="S39">
-        <v>0</v>
-      </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
-      <c r="U39">
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="5">
-        <v>1.5745341614899999</v>
-      </c>
-      <c r="C44" s="5">
-        <v>3.1490683229799998</v>
-      </c>
-      <c r="D44">
+      <c r="B41">
+        <v>1.4347826087</v>
+      </c>
+      <c r="C41">
+        <v>2.8695652173899999</v>
+      </c>
+      <c r="D41">
+        <v>1.4347826087</v>
+      </c>
+      <c r="E41">
+        <v>1.4347826087</v>
+      </c>
+      <c r="F41">
+        <v>1.3043478260900001</v>
+      </c>
+      <c r="G41">
+        <v>1.3043478260900001</v>
+      </c>
+      <c r="H41">
+        <v>0.13043478260899999</v>
+      </c>
+      <c r="I41">
+        <v>1.3043478260900001</v>
+      </c>
+      <c r="J41">
+        <v>12</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>1.4347826087</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>12</v>
+      </c>
+      <c r="P41">
+        <v>4.1739130434799998</v>
+      </c>
+      <c r="Q41">
+        <v>-1.4347826087</v>
+      </c>
+      <c r="R41">
+        <v>4.1739130434799998</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46">
+        <v>0.55334290608799996</v>
+      </c>
+      <c r="C46">
+        <v>0.27667145304399998</v>
+      </c>
+      <c r="D46">
+        <v>-1.1666666666700001</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>-1.5333333333300001</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="3">
+        <v>2.1521739130399999</v>
+      </c>
+      <c r="C47" s="3">
+        <v>4.3043478260899999</v>
+      </c>
+      <c r="D47">
         <v>0.71739130434800003</v>
       </c>
-      <c r="E44">
-        <v>0.71739130434800003</v>
-      </c>
-      <c r="F44">
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
         <v>0.65217391304299999</v>
       </c>
-      <c r="G44">
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>12</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>-10</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48">
+        <f>SUMPRODUCT(B46:U46,B47:U47)</f>
+        <v>0.54482381316062134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50">
+        <f>SUMPRODUCT(B46:U46,B49:U49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55">
+        <f>2*B32-D32-H32-I32-N32</f>
+        <v>3.5869565217319996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56">
+        <f>2*B32-F32-2*H32-I32-N32</f>
+        <v>3.6521739130370001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57">
+        <f>4.5*C32-2*B32+11.5*G32-10*I32</f>
+        <v>15.065217391325</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58">
+        <f>F32+2*H32+I32</f>
         <v>0.65217391304299999</v>
-      </c>
-      <c r="H44">
-        <v>6.5217391304300001E-2</v>
-      </c>
-      <c r="I44">
-        <v>0.65217391304299999</v>
-      </c>
-      <c r="J44">
-        <v>12</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44">
-        <v>1.5745341614899999</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-      <c r="N44">
-        <v>1.7142857142900001</v>
-      </c>
-      <c r="O44">
-        <v>12</v>
-      </c>
-      <c r="P44">
-        <v>2.0869565217399999</v>
-      </c>
-      <c r="Q44">
-        <v>-1.5745341614899999</v>
-      </c>
-      <c r="R44">
-        <v>2.0869565217399999</v>
-      </c>
-      <c r="S44">
-        <v>1.7142857142900001</v>
-      </c>
-      <c r="T44">
-        <v>0</v>
-      </c>
-      <c r="U44">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1721,7 +1883,7 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="2">
         <f>SUMPRODUCT(B3:P3,B$22:P$22)</f>
         <v>0</v>
       </c>
@@ -1733,8 +1895,8 @@
       <c r="L4">
         <v>-1</v>
       </c>
-      <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q22" si="0">SUMPRODUCT(B4:P4,B$22:P$22)</f>
+      <c r="Q4" s="2">
+        <f t="shared" ref="Q4:Q21" si="0">SUMPRODUCT(B4:P4,B$22:P$22)</f>
         <v>-10</v>
       </c>
     </row>
@@ -1754,7 +1916,7 @@
       <c r="P5">
         <v>-1</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="2">
         <f t="shared" si="0"/>
         <v>-7.000267032708507E-11</v>
       </c>
@@ -1766,12 +1928,12 @@
       <c r="P6">
         <v>1</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="2">
         <f t="shared" si="0"/>
         <v>43.011235955099998</v>
       </c>
       <c r="R6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1793,7 +1955,7 @@
       <c r="N7">
         <v>-1</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="2">
         <f t="shared" si="0"/>
         <v>4.000089148803454E-11</v>
       </c>
@@ -1808,12 +1970,12 @@
       <c r="N8">
         <v>1</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="R8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1835,7 +1997,7 @@
       <c r="M9">
         <v>-1</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="2">
         <f t="shared" si="0"/>
         <v>3.000044657142098E-11</v>
       </c>
@@ -1850,12 +2012,12 @@
       <c r="M10">
         <v>1</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="2">
         <f t="shared" si="0"/>
         <v>2.4269662921299999</v>
       </c>
       <c r="R10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1871,7 +2033,7 @@
       <c r="O11">
         <v>-1</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1883,12 +2045,12 @@
       <c r="O12">
         <v>1</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="2">
         <f t="shared" si="0"/>
         <v>22.2921348315</v>
       </c>
       <c r="R12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1904,7 +2066,7 @@
       <c r="K13">
         <v>-1</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="Q13" s="2">
         <f t="shared" si="0"/>
         <v>-3.000089066063083E-11</v>
       </c>
@@ -1922,7 +2084,7 @@
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q14" s="2">
         <f t="shared" si="0"/>
         <v>3.000089066063083E-11</v>
       </c>
@@ -1946,7 +2108,7 @@
       <c r="J15">
         <v>-1</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q15" s="2">
         <f t="shared" si="0"/>
         <v>9.99982319171977E-11</v>
       </c>
@@ -1970,7 +2132,7 @@
       <c r="J16">
         <v>1</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q16" s="2">
         <f t="shared" si="0"/>
         <v>-9.99982319171977E-11</v>
       </c>
@@ -1985,7 +2147,7 @@
       <c r="C17">
         <v>-1</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="Q17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2000,7 +2162,7 @@
       <c r="E18">
         <v>-1</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="Q18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2018,7 +2180,7 @@
       <c r="H19">
         <v>-1</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="Q19" s="2">
         <f t="shared" si="0"/>
         <v>-3.000044657142098E-11</v>
       </c>
@@ -2033,13 +2195,13 @@
       <c r="G20">
         <v>-1</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="Q20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q21" s="4">
+      <c r="Q21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2093,7 +2255,7 @@
       <c r="P22">
         <v>43.011235955099998</v>
       </c>
-      <c r="Q22" s="4"/>
+      <c r="Q22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MPStoCobraModel.py can now be used from the command line.
</commit_message>
<xml_diff>
--- a/Work/Excel/gx-fba examples.xlsx
+++ b/Work/Excel/gx-fba examples.xlsx
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,19 +1369,19 @@
         <v>46</v>
       </c>
       <c r="B34">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1390,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="B37">
         <f>SUMPRODUCT(B32:U32,B34:U34)</f>
-        <v>10.369565217390498</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>